<commit_message>
A possibility to add new tables to an existing .db file
</commit_message>
<xml_diff>
--- a/vocabulary_tester/words/ch9.xlsx
+++ b/vocabulary_tester/words/ch9.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.makipaa\Desktop\Opinnot\Japani\sanakoe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.makipaa\Desktop\git_omat\python-stuff\vocabulary_tester\words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572E5A6F-57C3-463B-8BC8-62FF7E09A646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510AFB17-AB72-41FD-A7DB-051A3C420783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
-    <t>Japani</t>
-  </si>
-  <si>
-    <t>Suomi</t>
-  </si>
-  <si>
     <t>みずうみ</t>
   </si>
   <si>
@@ -229,6 +223,12 @@
   </si>
   <si>
     <t>työ</t>
+  </si>
+  <si>
+    <t>japanese</t>
+  </si>
+  <si>
+    <t>finnish</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,322 +622,322 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>